<commit_message>
3rd and 4th models
</commit_message>
<xml_diff>
--- a/Project Handout/data.xlsx
+++ b/Project Handout/data.xlsx
@@ -455,10 +455,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>98.18750023841858</v>
+        <v>90.28499722480774</v>
       </c>
       <c r="C2" t="n">
-        <v>68.32000017166138</v>
+        <v>66.90000295639038</v>
       </c>
     </row>
   </sheetData>
@@ -499,10 +499,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>70.38250000000001</v>
+        <v>64.7075</v>
       </c>
       <c r="C2" t="n">
-        <v>53.08000000000001</v>
+        <v>53.3</v>
       </c>
     </row>
   </sheetData>
@@ -556,19 +556,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>52.87500000000001</v>
+        <v>50.575</v>
       </c>
       <c r="C2" t="n">
-        <v>0.05750000000000002</v>
+        <v>0.0115</v>
       </c>
       <c r="D2" t="n">
-        <v>0.5600835945663531</v>
+        <v>0.5323943661971831</v>
       </c>
       <c r="E2" t="n">
-        <v>0.268</v>
+        <v>0.0945</v>
       </c>
       <c r="F2" t="n">
-        <v>0.362529590801488</v>
+        <v>0.1605095541401274</v>
       </c>
     </row>
     <row r="3">
@@ -576,19 +576,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>57.45</v>
+        <v>55.375</v>
       </c>
       <c r="C3" t="n">
-        <v>0.149</v>
+        <v>0.1074999999999999</v>
       </c>
       <c r="D3" t="n">
-        <v>0.5507493188010899</v>
+        <v>0.537030657940062</v>
       </c>
       <c r="E3" t="n">
-        <v>0.8085</v>
+        <v>0.7795</v>
       </c>
       <c r="F3" t="n">
-        <v>0.6551863857374393</v>
+        <v>0.6359371813175607</v>
       </c>
     </row>
   </sheetData>
@@ -627,10 +627,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C2" t="n">
-        <v>0.12</v>
+        <v>0.24</v>
       </c>
     </row>
     <row r="3">
@@ -638,10 +638,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>50.58823529411764</v>
+        <v>47.05882352941176</v>
       </c>
       <c r="C3" t="n">
-        <v>0.2</v>
+        <v>0.3411764705882353</v>
       </c>
     </row>
     <row r="4">
@@ -649,10 +649,10 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>43.02325581395349</v>
+        <v>48.83720930232558</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1279069767441861</v>
+        <v>0.313953488372093</v>
       </c>
     </row>
     <row r="5">
@@ -660,10 +660,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>37.5</v>
+        <v>44.31818181818182</v>
       </c>
       <c r="C5" t="n">
-        <v>0.25</v>
+        <v>0.4318181818181818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>